<commit_message>
Listados listos del 8 de agosto de 2024
</commit_message>
<xml_diff>
--- a/Agosto/08 agosto/lazaro cardenas/PLANTILLA LISTA DE ASPIRANTES_LÁZARO CÁRDENAS 2024 SEGUNDO EXAMEN.xlsx
+++ b/Agosto/08 agosto/lazaro cardenas/PLANTILLA LISTA DE ASPIRANTES_LÁZARO CÁRDENAS 2024 SEGUNDO EXAMEN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27930"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollo 2022\Servicio Social 2022\01 Desarrollo - S Social 2024\EVALUATEC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proyecto01TICs\Documents\Evaluatec2024\Agosto\08 agosto\lazaro cardenas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E146122E-8E85-4D98-A3FE-2E3751B8C4C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABF79BD-183E-4D74-ACAF-01BF46C14528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D610CFFB-2790-104B-A52B-2B33694C28D9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{D610CFFB-2790-104B-A52B-2B33694C28D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1425,7 +1425,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1675,19 +1675,16 @@
     <cellStyle name="Hyperlink" xfId="2" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Arial Nova Cond"/>
-        <family val="2"/>
-        <scheme val="none"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1700,7 +1697,20 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="164" formatCode="h:mm\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Arial Nova Cond"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="h:mm\ AM/PM"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1714,7 +1724,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+      <numFmt numFmtId="164" formatCode="h:mm\ AM/PM"/>
     </dxf>
     <dxf>
       <font>
@@ -1727,7 +1737,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
       <font>
@@ -1852,29 +1862,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5925BC7A-0E73-734D-A0C9-B8A68F88FF64}" name="Tabla2" displayName="Tabla2" ref="A4:K469" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5925BC7A-0E73-734D-A0C9-B8A68F88FF64}" name="Tabla2" displayName="Tabla2" ref="A4:K469" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A4:K469" xr:uid="{5925BC7A-0E73-734D-A0C9-B8A68F88FF64}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:K469">
+    <sortCondition ref="E4:E469"/>
+  </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F5111305-CA2B-DF41-BA05-5C9A177B7523}" name=" FICHA" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{D956ADB6-2882-CB4B-9C6B-032AC358A5C1}" name="NOMBRE ASPIRANTE" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{0108DA77-7D27-7A48-8EFD-9B1F2B8F8E02}" name="CURP" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{12ECD994-2599-D747-9343-DEBBC900F696}" name="CORREO ELECTRONICO" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{2CF83F94-7C47-E74B-A32A-851420E76EC2}" name="CLAVE CARRERA" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{EC8B66B2-D538-484E-9EC1-54F93F611149}" name="CARRERA" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{A03F9403-44DC-3442-924E-BEF260777F9E}" name="VERSION" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{7AF8570F-2BED-A94F-B1CD-180258ABC8CA}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{FD3E5F78-2C8E-FB4D-924C-FA114DEF91F1}" name="HORA APLICACIÓN OFICIAL" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{B5C530FC-6A39-C746-86DE-949977537C53}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{44D56D16-D5EE-CE4F-8BAC-A3A00266F657}" name="AULA" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F5111305-CA2B-DF41-BA05-5C9A177B7523}" name=" FICHA" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{D956ADB6-2882-CB4B-9C6B-032AC358A5C1}" name="NOMBRE ASPIRANTE" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{0108DA77-7D27-7A48-8EFD-9B1F2B8F8E02}" name="CURP" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{12ECD994-2599-D747-9343-DEBBC900F696}" name="CORREO ELECTRONICO" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{2CF83F94-7C47-E74B-A32A-851420E76EC2}" name="CLAVE CARRERA" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{EC8B66B2-D538-484E-9EC1-54F93F611149}" name="CARRERA" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{A03F9403-44DC-3442-924E-BEF260777F9E}" name="VERSION" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{7AF8570F-2BED-A94F-B1CD-180258ABC8CA}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{FD3E5F78-2C8E-FB4D-924C-FA114DEF91F1}" name="HORA APLICACIÓN OFICIAL" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{B5C530FC-6A39-C746-86DE-949977537C53}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{44D56D16-D5EE-CE4F-8BAC-A3A00266F657}" name="AULA" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1912,7 +1925,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2018,7 +2031,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2160,7 +2173,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2170,11 +2183,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D137AA-41E5-5140-AC23-8A814C9A306A}">
   <dimension ref="A1:M469"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="C122" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E134" sqref="E134:F134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="39.5" style="1" bestFit="1" customWidth="1"/>
@@ -2190,12 +2203,12 @@
     <col min="12" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J1" s="28" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="21" customHeight="1" thickBot="1">
+    <row r="2" spans="1:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="27" t="s">
         <v>1</v>
       </c>
@@ -2206,10 +2219,10 @@
       <c r="H2" s="27"/>
       <c r="J2" s="28"/>
     </row>
-    <row r="3" spans="1:13" ht="16.5" thickTop="1">
+    <row r="3" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="J3" s="28"/>
     </row>
-    <row r="4" spans="1:13" ht="31.5">
+    <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2244,7 +2257,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>20240596</v>
       </c>
@@ -2282,7 +2295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>20240601</v>
       </c>
@@ -2321,7 +2334,7 @@
       </c>
       <c r="M6" s="26"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>20240618</v>
       </c>
@@ -2359,7 +2372,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>20240672</v>
       </c>
@@ -2397,7 +2410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>20240674</v>
       </c>
@@ -2435,7 +2448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>20240684</v>
       </c>
@@ -2473,7 +2486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>20240685</v>
       </c>
@@ -2511,7 +2524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>20240594</v>
       </c>
@@ -2549,7 +2562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>20240597</v>
       </c>
@@ -2587,7 +2600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>20240645</v>
       </c>
@@ -2625,7 +2638,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>20240667</v>
       </c>
@@ -2663,7 +2676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>20240679</v>
       </c>
@@ -2701,7 +2714,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>20240683</v>
       </c>
@@ -2739,7 +2752,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>20240696</v>
       </c>
@@ -2777,7 +2790,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>20240397</v>
       </c>
@@ -2815,7 +2828,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>20240416</v>
       </c>
@@ -2853,7 +2866,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>20240421</v>
       </c>
@@ -2891,7 +2904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>20240484</v>
       </c>
@@ -2929,7 +2942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>20240498</v>
       </c>
@@ -2967,7 +2980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>20240499</v>
       </c>
@@ -3005,7 +3018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>20240603</v>
       </c>
@@ -3043,7 +3056,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>20240611</v>
       </c>
@@ -3081,7 +3094,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>20240628</v>
       </c>
@@ -3119,7 +3132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>20240632</v>
       </c>
@@ -3157,7 +3170,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>20240637</v>
       </c>
@@ -3195,7 +3208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>20240640</v>
       </c>
@@ -3233,7 +3246,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>20240643</v>
       </c>
@@ -3271,7 +3284,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>20240649</v>
       </c>
@@ -3309,7 +3322,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>20240651</v>
       </c>
@@ -3347,7 +3360,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>20240659</v>
       </c>
@@ -3385,7 +3398,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>20240666</v>
       </c>
@@ -3423,7 +3436,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>20240670</v>
       </c>
@@ -3461,7 +3474,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>20240675</v>
       </c>
@@ -3499,7 +3512,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>20240692</v>
       </c>
@@ -3537,7 +3550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>20240698</v>
       </c>
@@ -3575,7 +3588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>20240703</v>
       </c>
@@ -3613,7 +3626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>20240705</v>
       </c>
@@ -3651,7 +3664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>20240706</v>
       </c>
@@ -3689,7 +3702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>20240707</v>
       </c>
@@ -3727,7 +3740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>20240037</v>
       </c>
@@ -3765,7 +3778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>20240473</v>
       </c>
@@ -3803,7 +3816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>20240561</v>
       </c>
@@ -3841,7 +3854,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>20240605</v>
       </c>
@@ -3879,7 +3892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>20240610</v>
       </c>
@@ -3917,7 +3930,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>20240699</v>
       </c>
@@ -3955,7 +3968,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <v>20240300</v>
       </c>
@@ -3993,7 +4006,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>20240326</v>
       </c>
@@ -4031,7 +4044,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>20240407</v>
       </c>
@@ -4069,7 +4082,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
         <v>20240453</v>
       </c>
@@ -4107,7 +4120,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
         <v>20240490</v>
       </c>
@@ -4145,7 +4158,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
         <v>20240517</v>
       </c>
@@ -4183,7 +4196,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <v>20240554</v>
       </c>
@@ -4221,7 +4234,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
         <v>20240599</v>
       </c>
@@ -4259,7 +4272,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
         <v>20240604</v>
       </c>
@@ -4297,7 +4310,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
         <v>20240629</v>
       </c>
@@ -4335,7 +4348,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
         <v>20240635</v>
       </c>
@@ -4373,7 +4386,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
         <v>20240636</v>
       </c>
@@ -4411,7 +4424,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
         <v>20240641</v>
       </c>
@@ -4449,7 +4462,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
         <v>20240652</v>
       </c>
@@ -4487,7 +4500,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
         <v>20240653</v>
       </c>
@@ -4525,7 +4538,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
         <v>20240654</v>
       </c>
@@ -4563,7 +4576,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>20240657</v>
       </c>
@@ -4601,7 +4614,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
         <v>20240668</v>
       </c>
@@ -4639,7 +4652,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
         <v>20240669</v>
       </c>
@@ -4677,7 +4690,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
         <v>20240682</v>
       </c>
@@ -4715,7 +4728,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
         <v>20240688</v>
       </c>
@@ -4753,7 +4766,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <v>20240690</v>
       </c>
@@ -4791,7 +4804,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>20240710</v>
       </c>
@@ -4829,7 +4842,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>20240711</v>
       </c>
@@ -4867,7 +4880,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="9">
         <v>20240712</v>
       </c>
@@ -4905,7 +4918,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
         <v>20240713</v>
       </c>
@@ -4943,7 +4956,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>20240714</v>
       </c>
@@ -4981,7 +4994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <v>20240064</v>
       </c>
@@ -5019,7 +5032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <v>20240079</v>
       </c>
@@ -5057,7 +5070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
         <v>20240350</v>
       </c>
@@ -5095,7 +5108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
         <v>20240609</v>
       </c>
@@ -5133,7 +5146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>20240616</v>
       </c>
@@ -5171,7 +5184,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>20240619</v>
       </c>
@@ -5209,7 +5222,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
         <v>20240621</v>
       </c>
@@ -5247,7 +5260,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:12">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>20240625</v>
       </c>
@@ -5285,7 +5298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:12">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>20240627</v>
       </c>
@@ -5323,7 +5336,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:12">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
         <v>20240633</v>
       </c>
@@ -5361,7 +5374,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:12">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <v>20240646</v>
       </c>
@@ -5399,7 +5412,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:12">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <v>20240648</v>
       </c>
@@ -5437,7 +5450,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:12">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <v>20240655</v>
       </c>
@@ -5475,7 +5488,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:12">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>20240661</v>
       </c>
@@ -5513,7 +5526,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:12">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
         <v>20240665</v>
       </c>
@@ -5551,7 +5564,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:12">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
         <v>20240678</v>
       </c>
@@ -5589,7 +5602,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:12">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
         <v>20240686</v>
       </c>
@@ -5627,7 +5640,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="9">
         <v>20240687</v>
       </c>
@@ -5665,7 +5678,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:12">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="9">
         <v>20240693</v>
       </c>
@@ -5703,7 +5716,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:12">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>20240695</v>
       </c>
@@ -5741,7 +5754,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:12">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="9">
         <v>20240697</v>
       </c>
@@ -5779,7 +5792,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="98" spans="1:12">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="9">
         <v>20240700</v>
       </c>
@@ -5817,7 +5830,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:12">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="9">
         <v>20240701</v>
       </c>
@@ -5855,7 +5868,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="1:12">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="9">
         <v>20240702</v>
       </c>
@@ -5893,7 +5906,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:12">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
         <v>20240715</v>
       </c>
@@ -5931,7 +5944,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:12">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="9">
         <v>20240107</v>
       </c>
@@ -5969,7 +5982,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="103" spans="1:12">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="9">
         <v>20240122</v>
       </c>
@@ -6007,7 +6020,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="104" spans="1:12">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="9">
         <v>20240140</v>
       </c>
@@ -6045,7 +6058,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="105" spans="1:12">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="9">
         <v>20240492</v>
       </c>
@@ -6083,7 +6096,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="106" spans="1:12">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="9">
         <v>20240493</v>
       </c>
@@ -6121,7 +6134,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:12">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="9">
         <v>20240516</v>
       </c>
@@ -6159,7 +6172,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:12">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="9">
         <v>20240598</v>
       </c>
@@ -6197,7 +6210,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="109" spans="1:12">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="9">
         <v>20240606</v>
       </c>
@@ -6235,7 +6248,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="110" spans="1:12">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="9">
         <v>20240614</v>
       </c>
@@ -6273,7 +6286,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="111" spans="1:12">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="9">
         <v>20240622</v>
       </c>
@@ -6311,7 +6324,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="112" spans="1:12">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="9">
         <v>20240624</v>
       </c>
@@ -6349,7 +6362,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="113" spans="1:12">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="9">
         <v>20240626</v>
       </c>
@@ -6387,7 +6400,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="114" spans="1:12">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="9">
         <v>20240631</v>
       </c>
@@ -6425,7 +6438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:12">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="9">
         <v>20240642</v>
       </c>
@@ -6463,7 +6476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:12">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="9">
         <v>20240644</v>
       </c>
@@ -6501,7 +6514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:12">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="9">
         <v>20240663</v>
       </c>
@@ -6539,7 +6552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:12">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="9">
         <v>20240671</v>
       </c>
@@ -6577,7 +6590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:12">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="9">
         <v>20240691</v>
       </c>
@@ -6615,7 +6628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="1:12">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="9">
         <v>20240379</v>
       </c>
@@ -6653,7 +6666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:12">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="9">
         <v>20240612</v>
       </c>
@@ -6691,7 +6704,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:12">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="9">
         <v>20240615</v>
       </c>
@@ -6729,7 +6742,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:12">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="9">
         <v>20240623</v>
       </c>
@@ -6767,7 +6780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="9">
         <v>20240639</v>
       </c>
@@ -6805,7 +6818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="125" spans="1:12">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="9">
         <v>20240647</v>
       </c>
@@ -6843,7 +6856,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:12">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="9">
         <v>20240658</v>
       </c>
@@ -6881,7 +6894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="127" spans="1:12">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="9">
         <v>20240664</v>
       </c>
@@ -6919,7 +6932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="128" spans="1:12">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="9">
         <v>20240689</v>
       </c>
@@ -6957,7 +6970,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:12">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="9">
         <v>20240694</v>
       </c>
@@ -6995,7 +7008,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="130" spans="1:12">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="9">
         <v>20240595</v>
       </c>
@@ -7033,7 +7046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:12">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="9">
         <v>20240600</v>
       </c>
@@ -7071,7 +7084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:12">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="9">
         <v>20240607</v>
       </c>
@@ -7109,7 +7122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:12">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="9">
         <v>20240608</v>
       </c>
@@ -7147,7 +7160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:12">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="9">
         <v>20240613</v>
       </c>
@@ -7185,7 +7198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:12">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="9">
         <v>20240617</v>
       </c>
@@ -7223,7 +7236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:12">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="9">
         <v>20240634</v>
       </c>
@@ -7261,7 +7274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:12">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="9">
         <v>20240638</v>
       </c>
@@ -7299,7 +7312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="138" spans="1:12">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="9">
         <v>20240660</v>
       </c>
@@ -7337,7 +7350,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:12">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="9">
         <v>20240662</v>
       </c>
@@ -7375,7 +7388,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:12">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="9">
         <v>20240673</v>
       </c>
@@ -7413,7 +7426,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:12">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="9">
         <v>20240677</v>
       </c>
@@ -7451,7 +7464,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="1:12">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="9">
         <v>20240680</v>
       </c>
@@ -7489,7 +7502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="143" spans="1:12">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="9">
         <v>20240681</v>
       </c>
@@ -7527,7 +7540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="144" spans="1:12">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="9">
         <v>20240704</v>
       </c>
@@ -7565,7 +7578,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:12">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="9">
         <v>20240718</v>
       </c>
@@ -7603,7 +7616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="146" spans="1:12">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="9"/>
       <c r="B146" s="18"/>
       <c r="C146" s="19"/>
@@ -7616,7 +7629,7 @@
       <c r="J146" s="7"/>
       <c r="K146" s="6"/>
     </row>
-    <row r="147" spans="1:12">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="9"/>
       <c r="B147" s="18"/>
       <c r="C147" s="19"/>
@@ -7629,7 +7642,7 @@
       <c r="J147" s="7"/>
       <c r="K147" s="6"/>
     </row>
-    <row r="148" spans="1:12">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="9"/>
       <c r="B148" s="18"/>
       <c r="C148" s="19"/>
@@ -7642,7 +7655,7 @@
       <c r="J148" s="7"/>
       <c r="K148" s="6"/>
     </row>
-    <row r="149" spans="1:12">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="9"/>
       <c r="B149" s="18"/>
       <c r="C149" s="19"/>
@@ -7655,7 +7668,7 @@
       <c r="J149" s="7"/>
       <c r="K149" s="6"/>
     </row>
-    <row r="150" spans="1:12">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="9"/>
       <c r="B150" s="18"/>
       <c r="C150" s="19"/>
@@ -7668,7 +7681,7 @@
       <c r="J150" s="7"/>
       <c r="K150" s="6"/>
     </row>
-    <row r="151" spans="1:12">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="9"/>
       <c r="B151" s="18"/>
       <c r="C151" s="19"/>
@@ -7681,7 +7694,7 @@
       <c r="J151" s="7"/>
       <c r="K151" s="6"/>
     </row>
-    <row r="152" spans="1:12">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="9"/>
       <c r="B152" s="18"/>
       <c r="C152" s="19"/>
@@ -7694,7 +7707,7 @@
       <c r="J152" s="7"/>
       <c r="K152" s="6"/>
     </row>
-    <row r="153" spans="1:12">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="9"/>
       <c r="B153" s="18"/>
       <c r="C153" s="19"/>
@@ -7707,7 +7720,7 @@
       <c r="J153" s="7"/>
       <c r="K153" s="6"/>
     </row>
-    <row r="154" spans="1:12">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="9"/>
       <c r="B154" s="18"/>
       <c r="C154" s="19"/>
@@ -7720,7 +7733,7 @@
       <c r="J154" s="7"/>
       <c r="K154" s="6"/>
     </row>
-    <row r="155" spans="1:12">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="9"/>
       <c r="B155" s="18"/>
       <c r="C155" s="19"/>
@@ -7733,7 +7746,7 @@
       <c r="J155" s="7"/>
       <c r="K155" s="6"/>
     </row>
-    <row r="156" spans="1:12">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="9"/>
       <c r="B156" s="18"/>
       <c r="C156" s="19"/>
@@ -7746,7 +7759,7 @@
       <c r="J156" s="7"/>
       <c r="K156" s="6"/>
     </row>
-    <row r="157" spans="1:12">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="9"/>
       <c r="B157" s="18"/>
       <c r="C157" s="19"/>
@@ -7759,7 +7772,7 @@
       <c r="J157" s="7"/>
       <c r="K157" s="6"/>
     </row>
-    <row r="158" spans="1:12">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="9"/>
       <c r="B158" s="18"/>
       <c r="C158" s="19"/>
@@ -7772,7 +7785,7 @@
       <c r="J158" s="7"/>
       <c r="K158" s="6"/>
     </row>
-    <row r="159" spans="1:12">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="9"/>
       <c r="B159" s="18"/>
       <c r="C159" s="19"/>
@@ -7785,7 +7798,7 @@
       <c r="J159" s="7"/>
       <c r="K159" s="6"/>
     </row>
-    <row r="160" spans="1:12">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="9"/>
       <c r="B160" s="18"/>
       <c r="C160" s="19"/>
@@ -7798,7 +7811,7 @@
       <c r="J160" s="7"/>
       <c r="K160" s="6"/>
     </row>
-    <row r="161" spans="1:11">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="9"/>
       <c r="B161" s="18"/>
       <c r="C161" s="19"/>
@@ -7811,7 +7824,7 @@
       <c r="J161" s="7"/>
       <c r="K161" s="6"/>
     </row>
-    <row r="162" spans="1:11">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="9"/>
       <c r="B162" s="18"/>
       <c r="C162" s="19"/>
@@ -7824,7 +7837,7 @@
       <c r="J162" s="7"/>
       <c r="K162" s="6"/>
     </row>
-    <row r="163" spans="1:11">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="9"/>
       <c r="B163" s="18"/>
       <c r="C163" s="19"/>
@@ -7837,7 +7850,7 @@
       <c r="J163" s="7"/>
       <c r="K163" s="6"/>
     </row>
-    <row r="164" spans="1:11">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="9"/>
       <c r="B164" s="18"/>
       <c r="C164" s="19"/>
@@ -7850,7 +7863,7 @@
       <c r="J164" s="7"/>
       <c r="K164" s="6"/>
     </row>
-    <row r="165" spans="1:11">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="9"/>
       <c r="B165" s="18"/>
       <c r="C165" s="19"/>
@@ -7863,7 +7876,7 @@
       <c r="J165" s="7"/>
       <c r="K165" s="6"/>
     </row>
-    <row r="166" spans="1:11">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="9"/>
       <c r="B166" s="18"/>
       <c r="C166" s="19"/>
@@ -7876,7 +7889,7 @@
       <c r="J166" s="7"/>
       <c r="K166" s="6"/>
     </row>
-    <row r="167" spans="1:11">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="9"/>
       <c r="B167" s="18"/>
       <c r="C167" s="19"/>
@@ -7889,7 +7902,7 @@
       <c r="J167" s="7"/>
       <c r="K167" s="6"/>
     </row>
-    <row r="168" spans="1:11">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="9"/>
       <c r="B168" s="18"/>
       <c r="C168" s="19"/>
@@ -7902,7 +7915,7 @@
       <c r="J168" s="7"/>
       <c r="K168" s="6"/>
     </row>
-    <row r="169" spans="1:11">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="9"/>
       <c r="B169" s="18"/>
       <c r="C169" s="19"/>
@@ -7915,7 +7928,7 @@
       <c r="J169" s="7"/>
       <c r="K169" s="6"/>
     </row>
-    <row r="170" spans="1:11">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="9"/>
       <c r="B170" s="18"/>
       <c r="C170" s="19"/>
@@ -7928,7 +7941,7 @@
       <c r="J170" s="7"/>
       <c r="K170" s="6"/>
     </row>
-    <row r="171" spans="1:11">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="9"/>
       <c r="B171" s="18"/>
       <c r="C171" s="19"/>
@@ -7941,7 +7954,7 @@
       <c r="J171" s="7"/>
       <c r="K171" s="6"/>
     </row>
-    <row r="172" spans="1:11">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="9"/>
       <c r="B172" s="18"/>
       <c r="C172" s="19"/>
@@ -7954,7 +7967,7 @@
       <c r="J172" s="7"/>
       <c r="K172" s="6"/>
     </row>
-    <row r="173" spans="1:11">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="9"/>
       <c r="B173" s="18"/>
       <c r="C173" s="19"/>
@@ -7967,7 +7980,7 @@
       <c r="J173" s="7"/>
       <c r="K173" s="6"/>
     </row>
-    <row r="174" spans="1:11">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="9"/>
       <c r="B174" s="18"/>
       <c r="C174" s="19"/>
@@ -7980,7 +7993,7 @@
       <c r="J174" s="7"/>
       <c r="K174" s="6"/>
     </row>
-    <row r="175" spans="1:11">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="9"/>
       <c r="B175" s="18"/>
       <c r="C175" s="19"/>
@@ -7993,7 +8006,7 @@
       <c r="J175" s="7"/>
       <c r="K175" s="6"/>
     </row>
-    <row r="176" spans="1:11">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="9"/>
       <c r="B176" s="18"/>
       <c r="C176" s="19"/>
@@ -8006,7 +8019,7 @@
       <c r="J176" s="7"/>
       <c r="K176" s="6"/>
     </row>
-    <row r="177" spans="1:11">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="9"/>
       <c r="B177" s="18"/>
       <c r="C177" s="19"/>
@@ -8019,7 +8032,7 @@
       <c r="J177" s="7"/>
       <c r="K177" s="6"/>
     </row>
-    <row r="178" spans="1:11">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="9"/>
       <c r="B178" s="18"/>
       <c r="C178" s="19"/>
@@ -8032,7 +8045,7 @@
       <c r="J178" s="7"/>
       <c r="K178" s="6"/>
     </row>
-    <row r="179" spans="1:11">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="9"/>
       <c r="B179" s="18"/>
       <c r="C179" s="19"/>
@@ -8045,7 +8058,7 @@
       <c r="J179" s="7"/>
       <c r="K179" s="6"/>
     </row>
-    <row r="180" spans="1:11">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="9"/>
       <c r="B180" s="18"/>
       <c r="C180" s="19"/>
@@ -8058,7 +8071,7 @@
       <c r="J180" s="7"/>
       <c r="K180" s="6"/>
     </row>
-    <row r="181" spans="1:11">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="9"/>
       <c r="B181" s="18"/>
       <c r="C181" s="19"/>
@@ -8071,7 +8084,7 @@
       <c r="J181" s="7"/>
       <c r="K181" s="6"/>
     </row>
-    <row r="182" spans="1:11">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="9"/>
       <c r="B182" s="18"/>
       <c r="C182" s="19"/>
@@ -8084,7 +8097,7 @@
       <c r="J182" s="7"/>
       <c r="K182" s="6"/>
     </row>
-    <row r="183" spans="1:11">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="9"/>
       <c r="B183" s="18"/>
       <c r="C183" s="19"/>
@@ -8097,7 +8110,7 @@
       <c r="J183" s="7"/>
       <c r="K183" s="6"/>
     </row>
-    <row r="184" spans="1:11">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="9"/>
       <c r="B184" s="18"/>
       <c r="C184" s="19"/>
@@ -8110,7 +8123,7 @@
       <c r="J184" s="7"/>
       <c r="K184" s="6"/>
     </row>
-    <row r="185" spans="1:11">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="9"/>
       <c r="B185" s="18"/>
       <c r="C185" s="19"/>
@@ -8123,7 +8136,7 @@
       <c r="J185" s="7"/>
       <c r="K185" s="6"/>
     </row>
-    <row r="186" spans="1:11">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="9"/>
       <c r="B186" s="18"/>
       <c r="C186" s="19"/>
@@ -8136,7 +8149,7 @@
       <c r="J186" s="7"/>
       <c r="K186" s="6"/>
     </row>
-    <row r="187" spans="1:11">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="9"/>
       <c r="B187" s="18"/>
       <c r="C187" s="19"/>
@@ -8149,7 +8162,7 @@
       <c r="J187" s="7"/>
       <c r="K187" s="6"/>
     </row>
-    <row r="188" spans="1:11">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="9"/>
       <c r="B188" s="18"/>
       <c r="C188" s="19"/>
@@ -8162,7 +8175,7 @@
       <c r="J188" s="7"/>
       <c r="K188" s="6"/>
     </row>
-    <row r="189" spans="1:11">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="9"/>
       <c r="B189" s="18"/>
       <c r="C189" s="19"/>
@@ -8175,7 +8188,7 @@
       <c r="J189" s="7"/>
       <c r="K189" s="6"/>
     </row>
-    <row r="190" spans="1:11">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="9"/>
       <c r="B190" s="18"/>
       <c r="C190" s="19"/>
@@ -8188,7 +8201,7 @@
       <c r="J190" s="7"/>
       <c r="K190" s="6"/>
     </row>
-    <row r="191" spans="1:11">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="9"/>
       <c r="B191" s="18"/>
       <c r="C191" s="19"/>
@@ -8201,7 +8214,7 @@
       <c r="J191" s="7"/>
       <c r="K191" s="6"/>
     </row>
-    <row r="192" spans="1:11">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="9"/>
       <c r="B192" s="18"/>
       <c r="C192" s="19"/>
@@ -8214,7 +8227,7 @@
       <c r="J192" s="7"/>
       <c r="K192" s="6"/>
     </row>
-    <row r="193" spans="1:11">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="9"/>
       <c r="B193" s="18"/>
       <c r="C193" s="19"/>
@@ -8227,7 +8240,7 @@
       <c r="J193" s="7"/>
       <c r="K193" s="6"/>
     </row>
-    <row r="194" spans="1:11">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="9"/>
       <c r="B194" s="18"/>
       <c r="C194" s="19"/>
@@ -8240,7 +8253,7 @@
       <c r="J194" s="7"/>
       <c r="K194" s="6"/>
     </row>
-    <row r="195" spans="1:11">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="9"/>
       <c r="B195" s="18"/>
       <c r="C195" s="19"/>
@@ -8253,7 +8266,7 @@
       <c r="J195" s="7"/>
       <c r="K195" s="6"/>
     </row>
-    <row r="196" spans="1:11">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="9"/>
       <c r="B196" s="18"/>
       <c r="C196" s="19"/>
@@ -8266,7 +8279,7 @@
       <c r="J196" s="7"/>
       <c r="K196" s="6"/>
     </row>
-    <row r="197" spans="1:11">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="9"/>
       <c r="B197" s="18"/>
       <c r="C197" s="19"/>
@@ -8279,7 +8292,7 @@
       <c r="J197" s="7"/>
       <c r="K197" s="6"/>
     </row>
-    <row r="198" spans="1:11">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="9"/>
       <c r="B198" s="18"/>
       <c r="C198" s="19"/>
@@ -8292,7 +8305,7 @@
       <c r="J198" s="7"/>
       <c r="K198" s="6"/>
     </row>
-    <row r="199" spans="1:11">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="9"/>
       <c r="B199" s="18"/>
       <c r="C199" s="19"/>
@@ -8305,7 +8318,7 @@
       <c r="J199" s="7"/>
       <c r="K199" s="6"/>
     </row>
-    <row r="200" spans="1:11">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="9"/>
       <c r="B200" s="18"/>
       <c r="C200" s="19"/>
@@ -8318,7 +8331,7 @@
       <c r="J200" s="7"/>
       <c r="K200" s="6"/>
     </row>
-    <row r="201" spans="1:11">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="9"/>
       <c r="B201" s="18"/>
       <c r="C201" s="19"/>
@@ -8331,7 +8344,7 @@
       <c r="J201" s="7"/>
       <c r="K201" s="6"/>
     </row>
-    <row r="202" spans="1:11">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="9"/>
       <c r="B202" s="18"/>
       <c r="C202" s="19"/>
@@ -8344,7 +8357,7 @@
       <c r="J202" s="7"/>
       <c r="K202" s="6"/>
     </row>
-    <row r="203" spans="1:11">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="9"/>
       <c r="B203" s="18"/>
       <c r="C203" s="19"/>
@@ -8357,7 +8370,7 @@
       <c r="J203" s="7"/>
       <c r="K203" s="6"/>
     </row>
-    <row r="204" spans="1:11">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="9"/>
       <c r="B204" s="18"/>
       <c r="C204" s="19"/>
@@ -8370,7 +8383,7 @@
       <c r="J204" s="7"/>
       <c r="K204" s="6"/>
     </row>
-    <row r="205" spans="1:11">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="9"/>
       <c r="B205" s="18"/>
       <c r="C205" s="19"/>
@@ -8383,7 +8396,7 @@
       <c r="J205" s="7"/>
       <c r="K205" s="6"/>
     </row>
-    <row r="206" spans="1:11">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="9"/>
       <c r="B206" s="18"/>
       <c r="C206" s="19"/>
@@ -8396,7 +8409,7 @@
       <c r="J206" s="7"/>
       <c r="K206" s="6"/>
     </row>
-    <row r="207" spans="1:11">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="9"/>
       <c r="B207" s="18"/>
       <c r="C207" s="19"/>
@@ -8409,7 +8422,7 @@
       <c r="J207" s="7"/>
       <c r="K207" s="6"/>
     </row>
-    <row r="208" spans="1:11">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="9"/>
       <c r="B208" s="18"/>
       <c r="C208" s="19"/>
@@ -8422,7 +8435,7 @@
       <c r="J208" s="7"/>
       <c r="K208" s="6"/>
     </row>
-    <row r="209" spans="1:11">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="9"/>
       <c r="B209" s="18"/>
       <c r="C209" s="19"/>
@@ -8435,7 +8448,7 @@
       <c r="J209" s="7"/>
       <c r="K209" s="6"/>
     </row>
-    <row r="210" spans="1:11">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="9"/>
       <c r="B210" s="18"/>
       <c r="C210" s="19"/>
@@ -8448,7 +8461,7 @@
       <c r="J210" s="7"/>
       <c r="K210" s="6"/>
     </row>
-    <row r="211" spans="1:11">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="9"/>
       <c r="B211" s="18"/>
       <c r="C211" s="19"/>
@@ -8461,7 +8474,7 @@
       <c r="J211" s="7"/>
       <c r="K211" s="6"/>
     </row>
-    <row r="212" spans="1:11">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="9"/>
       <c r="B212" s="18"/>
       <c r="C212" s="19"/>
@@ -8474,7 +8487,7 @@
       <c r="J212" s="7"/>
       <c r="K212" s="6"/>
     </row>
-    <row r="213" spans="1:11">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="9"/>
       <c r="B213" s="18"/>
       <c r="C213" s="19"/>
@@ -8487,7 +8500,7 @@
       <c r="J213" s="7"/>
       <c r="K213" s="6"/>
     </row>
-    <row r="214" spans="1:11">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="9"/>
       <c r="B214" s="18"/>
       <c r="C214" s="19"/>
@@ -8500,7 +8513,7 @@
       <c r="J214" s="7"/>
       <c r="K214" s="6"/>
     </row>
-    <row r="215" spans="1:11">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="9"/>
       <c r="B215" s="18"/>
       <c r="C215" s="19"/>
@@ -8513,7 +8526,7 @@
       <c r="J215" s="7"/>
       <c r="K215" s="6"/>
     </row>
-    <row r="216" spans="1:11">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="9"/>
       <c r="B216" s="18"/>
       <c r="C216" s="19"/>
@@ -8526,7 +8539,7 @@
       <c r="J216" s="7"/>
       <c r="K216" s="6"/>
     </row>
-    <row r="217" spans="1:11">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="9"/>
       <c r="B217" s="18"/>
       <c r="C217" s="19"/>
@@ -8539,7 +8552,7 @@
       <c r="J217" s="7"/>
       <c r="K217" s="6"/>
     </row>
-    <row r="218" spans="1:11">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="9"/>
       <c r="B218" s="18"/>
       <c r="C218" s="19"/>
@@ -8552,7 +8565,7 @@
       <c r="J218" s="7"/>
       <c r="K218" s="6"/>
     </row>
-    <row r="219" spans="1:11">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="9"/>
       <c r="B219" s="18"/>
       <c r="C219" s="19"/>
@@ -8565,7 +8578,7 @@
       <c r="J219" s="7"/>
       <c r="K219" s="6"/>
     </row>
-    <row r="220" spans="1:11">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" s="9"/>
       <c r="B220" s="18"/>
       <c r="C220" s="19"/>
@@ -8578,7 +8591,7 @@
       <c r="J220" s="7"/>
       <c r="K220" s="6"/>
     </row>
-    <row r="221" spans="1:11">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" s="9"/>
       <c r="B221" s="18"/>
       <c r="C221" s="19"/>
@@ -8591,7 +8604,7 @@
       <c r="J221" s="7"/>
       <c r="K221" s="6"/>
     </row>
-    <row r="222" spans="1:11">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" s="9"/>
       <c r="B222" s="18"/>
       <c r="C222" s="19"/>
@@ -8604,7 +8617,7 @@
       <c r="J222" s="7"/>
       <c r="K222" s="6"/>
     </row>
-    <row r="223" spans="1:11">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" s="9"/>
       <c r="B223" s="18"/>
       <c r="C223" s="19"/>
@@ -8617,7 +8630,7 @@
       <c r="J223" s="7"/>
       <c r="K223" s="6"/>
     </row>
-    <row r="224" spans="1:11">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="9"/>
       <c r="B224" s="18"/>
       <c r="C224" s="19"/>
@@ -8630,7 +8643,7 @@
       <c r="J224" s="7"/>
       <c r="K224" s="6"/>
     </row>
-    <row r="225" spans="1:11">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" s="9"/>
       <c r="B225" s="18"/>
       <c r="C225" s="19"/>
@@ -8643,7 +8656,7 @@
       <c r="J225" s="7"/>
       <c r="K225" s="6"/>
     </row>
-    <row r="226" spans="1:11">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" s="9"/>
       <c r="B226" s="18"/>
       <c r="C226" s="19"/>
@@ -8656,7 +8669,7 @@
       <c r="J226" s="7"/>
       <c r="K226" s="6"/>
     </row>
-    <row r="227" spans="1:11">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="9"/>
       <c r="B227" s="18"/>
       <c r="C227" s="19"/>
@@ -8669,7 +8682,7 @@
       <c r="J227" s="7"/>
       <c r="K227" s="6"/>
     </row>
-    <row r="228" spans="1:11">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" s="9"/>
       <c r="B228" s="18"/>
       <c r="C228" s="19"/>
@@ -8682,7 +8695,7 @@
       <c r="J228" s="7"/>
       <c r="K228" s="6"/>
     </row>
-    <row r="229" spans="1:11">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" s="9"/>
       <c r="B229" s="18"/>
       <c r="C229" s="19"/>
@@ -8695,7 +8708,7 @@
       <c r="J229" s="7"/>
       <c r="K229" s="6"/>
     </row>
-    <row r="230" spans="1:11">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="9"/>
       <c r="B230" s="18"/>
       <c r="C230" s="19"/>
@@ -8708,7 +8721,7 @@
       <c r="J230" s="7"/>
       <c r="K230" s="6"/>
     </row>
-    <row r="231" spans="1:11">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="9"/>
       <c r="B231" s="18"/>
       <c r="C231" s="19"/>
@@ -8721,7 +8734,7 @@
       <c r="J231" s="7"/>
       <c r="K231" s="6"/>
     </row>
-    <row r="232" spans="1:11">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" s="9"/>
       <c r="B232" s="18"/>
       <c r="C232" s="19"/>
@@ -8734,7 +8747,7 @@
       <c r="J232" s="7"/>
       <c r="K232" s="6"/>
     </row>
-    <row r="233" spans="1:11">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" s="9"/>
       <c r="B233" s="18"/>
       <c r="C233" s="19"/>
@@ -8747,7 +8760,7 @@
       <c r="J233" s="7"/>
       <c r="K233" s="6"/>
     </row>
-    <row r="234" spans="1:11">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" s="9"/>
       <c r="B234" s="18"/>
       <c r="C234" s="19"/>
@@ -8760,7 +8773,7 @@
       <c r="J234" s="7"/>
       <c r="K234" s="6"/>
     </row>
-    <row r="235" spans="1:11">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="9"/>
       <c r="B235" s="18"/>
       <c r="C235" s="19"/>
@@ -8773,7 +8786,7 @@
       <c r="J235" s="7"/>
       <c r="K235" s="6"/>
     </row>
-    <row r="236" spans="1:11">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" s="9"/>
       <c r="B236" s="18"/>
       <c r="C236" s="19"/>
@@ -8786,7 +8799,7 @@
       <c r="J236" s="7"/>
       <c r="K236" s="6"/>
     </row>
-    <row r="237" spans="1:11">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" s="9"/>
       <c r="B237" s="18"/>
       <c r="C237" s="19"/>
@@ -8799,7 +8812,7 @@
       <c r="J237" s="7"/>
       <c r="K237" s="6"/>
     </row>
-    <row r="238" spans="1:11">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" s="9"/>
       <c r="B238" s="18"/>
       <c r="C238" s="19"/>
@@ -8812,7 +8825,7 @@
       <c r="J238" s="7"/>
       <c r="K238" s="6"/>
     </row>
-    <row r="239" spans="1:11">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" s="9"/>
       <c r="B239" s="18"/>
       <c r="C239" s="19"/>
@@ -8825,7 +8838,7 @@
       <c r="J239" s="7"/>
       <c r="K239" s="6"/>
     </row>
-    <row r="240" spans="1:11">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" s="9"/>
       <c r="B240" s="18"/>
       <c r="C240" s="19"/>
@@ -8838,7 +8851,7 @@
       <c r="J240" s="7"/>
       <c r="K240" s="6"/>
     </row>
-    <row r="241" spans="1:11">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" s="9"/>
       <c r="B241" s="18"/>
       <c r="C241" s="19"/>
@@ -8851,7 +8864,7 @@
       <c r="J241" s="7"/>
       <c r="K241" s="6"/>
     </row>
-    <row r="242" spans="1:11">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" s="9"/>
       <c r="B242" s="18"/>
       <c r="C242" s="19"/>
@@ -8864,7 +8877,7 @@
       <c r="J242" s="7"/>
       <c r="K242" s="6"/>
     </row>
-    <row r="243" spans="1:11">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" s="9"/>
       <c r="B243" s="18"/>
       <c r="C243" s="19"/>
@@ -8877,7 +8890,7 @@
       <c r="J243" s="7"/>
       <c r="K243" s="6"/>
     </row>
-    <row r="244" spans="1:11">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" s="9"/>
       <c r="B244" s="18"/>
       <c r="C244" s="19"/>
@@ -8890,7 +8903,7 @@
       <c r="J244" s="7"/>
       <c r="K244" s="6"/>
     </row>
-    <row r="245" spans="1:11">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" s="9"/>
       <c r="B245" s="18"/>
       <c r="C245" s="19"/>
@@ -8903,7 +8916,7 @@
       <c r="J245" s="7"/>
       <c r="K245" s="6"/>
     </row>
-    <row r="246" spans="1:11">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" s="9"/>
       <c r="B246" s="18"/>
       <c r="C246" s="19"/>
@@ -8916,7 +8929,7 @@
       <c r="J246" s="7"/>
       <c r="K246" s="6"/>
     </row>
-    <row r="247" spans="1:11">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" s="9"/>
       <c r="B247" s="18"/>
       <c r="C247" s="19"/>
@@ -8929,7 +8942,7 @@
       <c r="J247" s="7"/>
       <c r="K247" s="6"/>
     </row>
-    <row r="248" spans="1:11">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" s="9"/>
       <c r="B248" s="18"/>
       <c r="C248" s="19"/>
@@ -8942,7 +8955,7 @@
       <c r="J248" s="7"/>
       <c r="K248" s="6"/>
     </row>
-    <row r="249" spans="1:11">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" s="9"/>
       <c r="B249" s="18"/>
       <c r="C249" s="19"/>
@@ -8955,7 +8968,7 @@
       <c r="J249" s="7"/>
       <c r="K249" s="6"/>
     </row>
-    <row r="250" spans="1:11">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" s="9"/>
       <c r="B250" s="18"/>
       <c r="C250" s="19"/>
@@ -8968,7 +8981,7 @@
       <c r="J250" s="7"/>
       <c r="K250" s="6"/>
     </row>
-    <row r="251" spans="1:11">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A251" s="9"/>
       <c r="B251" s="18"/>
       <c r="C251" s="19"/>
@@ -8981,7 +8994,7 @@
       <c r="J251" s="7"/>
       <c r="K251" s="6"/>
     </row>
-    <row r="252" spans="1:11">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252" s="9"/>
       <c r="B252" s="18"/>
       <c r="C252" s="19"/>
@@ -8994,7 +9007,7 @@
       <c r="J252" s="7"/>
       <c r="K252" s="6"/>
     </row>
-    <row r="253" spans="1:11">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A253" s="9"/>
       <c r="B253" s="18"/>
       <c r="C253" s="19"/>
@@ -9007,7 +9020,7 @@
       <c r="J253" s="7"/>
       <c r="K253" s="6"/>
     </row>
-    <row r="254" spans="1:11">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" s="9"/>
       <c r="B254" s="18"/>
       <c r="C254" s="19"/>
@@ -9020,7 +9033,7 @@
       <c r="J254" s="7"/>
       <c r="K254" s="6"/>
     </row>
-    <row r="255" spans="1:11">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" s="9"/>
       <c r="B255" s="18"/>
       <c r="C255" s="19"/>
@@ -9033,7 +9046,7 @@
       <c r="J255" s="7"/>
       <c r="K255" s="6"/>
     </row>
-    <row r="256" spans="1:11">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256" s="9"/>
       <c r="B256" s="18"/>
       <c r="C256" s="19"/>
@@ -9046,7 +9059,7 @@
       <c r="J256" s="7"/>
       <c r="K256" s="6"/>
     </row>
-    <row r="257" spans="1:11">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A257" s="9"/>
       <c r="B257" s="18"/>
       <c r="C257" s="19"/>
@@ -9059,7 +9072,7 @@
       <c r="J257" s="7"/>
       <c r="K257" s="6"/>
     </row>
-    <row r="258" spans="1:11">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" s="9"/>
       <c r="B258" s="18"/>
       <c r="C258" s="19"/>
@@ -9072,7 +9085,7 @@
       <c r="J258" s="7"/>
       <c r="K258" s="6"/>
     </row>
-    <row r="259" spans="1:11">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A259" s="9"/>
       <c r="B259" s="18"/>
       <c r="C259" s="19"/>
@@ -9085,7 +9098,7 @@
       <c r="J259" s="7"/>
       <c r="K259" s="6"/>
     </row>
-    <row r="260" spans="1:11">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260" s="9"/>
       <c r="B260" s="18"/>
       <c r="C260" s="19"/>
@@ -9098,7 +9111,7 @@
       <c r="J260" s="7"/>
       <c r="K260" s="6"/>
     </row>
-    <row r="261" spans="1:11">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A261" s="9"/>
       <c r="B261" s="18"/>
       <c r="C261" s="19"/>
@@ -9111,7 +9124,7 @@
       <c r="J261" s="7"/>
       <c r="K261" s="6"/>
     </row>
-    <row r="262" spans="1:11">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A262" s="9"/>
       <c r="B262" s="18"/>
       <c r="C262" s="19"/>
@@ -9124,7 +9137,7 @@
       <c r="J262" s="7"/>
       <c r="K262" s="6"/>
     </row>
-    <row r="263" spans="1:11">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A263" s="9"/>
       <c r="B263" s="18"/>
       <c r="C263" s="19"/>
@@ -9137,7 +9150,7 @@
       <c r="J263" s="7"/>
       <c r="K263" s="6"/>
     </row>
-    <row r="264" spans="1:11">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264" s="9"/>
       <c r="B264" s="18"/>
       <c r="C264" s="19"/>
@@ -9150,7 +9163,7 @@
       <c r="J264" s="7"/>
       <c r="K264" s="6"/>
     </row>
-    <row r="265" spans="1:11">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A265" s="9"/>
       <c r="B265" s="18"/>
       <c r="C265" s="19"/>
@@ -9163,7 +9176,7 @@
       <c r="J265" s="7"/>
       <c r="K265" s="6"/>
     </row>
-    <row r="266" spans="1:11">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A266" s="9"/>
       <c r="B266" s="18"/>
       <c r="C266" s="19"/>
@@ -9176,7 +9189,7 @@
       <c r="J266" s="7"/>
       <c r="K266" s="6"/>
     </row>
-    <row r="267" spans="1:11">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A267" s="9"/>
       <c r="B267" s="18"/>
       <c r="C267" s="19"/>
@@ -9189,7 +9202,7 @@
       <c r="J267" s="7"/>
       <c r="K267" s="6"/>
     </row>
-    <row r="268" spans="1:11">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A268" s="9"/>
       <c r="B268" s="18"/>
       <c r="C268" s="19"/>
@@ -9202,7 +9215,7 @@
       <c r="J268" s="7"/>
       <c r="K268" s="6"/>
     </row>
-    <row r="269" spans="1:11">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269" s="9"/>
       <c r="B269" s="18"/>
       <c r="C269" s="19"/>
@@ -9215,7 +9228,7 @@
       <c r="J269" s="7"/>
       <c r="K269" s="6"/>
     </row>
-    <row r="270" spans="1:11">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270" s="9"/>
       <c r="B270" s="18"/>
       <c r="C270" s="19"/>
@@ -9228,7 +9241,7 @@
       <c r="J270" s="7"/>
       <c r="K270" s="6"/>
     </row>
-    <row r="271" spans="1:11">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A271" s="9"/>
       <c r="B271" s="18"/>
       <c r="C271" s="19"/>
@@ -9241,7 +9254,7 @@
       <c r="J271" s="7"/>
       <c r="K271" s="6"/>
     </row>
-    <row r="272" spans="1:11">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" s="9"/>
       <c r="B272" s="18"/>
       <c r="C272" s="19"/>
@@ -9254,7 +9267,7 @@
       <c r="J272" s="7"/>
       <c r="K272" s="6"/>
     </row>
-    <row r="273" spans="1:11">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A273" s="9"/>
       <c r="B273" s="18"/>
       <c r="C273" s="19"/>
@@ -9267,7 +9280,7 @@
       <c r="J273" s="7"/>
       <c r="K273" s="6"/>
     </row>
-    <row r="274" spans="1:11">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274" s="9"/>
       <c r="B274" s="18"/>
       <c r="C274" s="19"/>
@@ -9280,7 +9293,7 @@
       <c r="J274" s="7"/>
       <c r="K274" s="6"/>
     </row>
-    <row r="275" spans="1:11">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A275" s="9"/>
       <c r="B275" s="18"/>
       <c r="C275" s="19"/>
@@ -9293,7 +9306,7 @@
       <c r="J275" s="7"/>
       <c r="K275" s="6"/>
     </row>
-    <row r="276" spans="1:11">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276" s="9"/>
       <c r="B276" s="18"/>
       <c r="C276" s="19"/>
@@ -9306,7 +9319,7 @@
       <c r="J276" s="7"/>
       <c r="K276" s="6"/>
     </row>
-    <row r="277" spans="1:11">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A277" s="9"/>
       <c r="B277" s="18"/>
       <c r="C277" s="19"/>
@@ -9319,7 +9332,7 @@
       <c r="J277" s="7"/>
       <c r="K277" s="6"/>
     </row>
-    <row r="278" spans="1:11">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" s="9"/>
       <c r="B278" s="18"/>
       <c r="C278" s="19"/>
@@ -9332,7 +9345,7 @@
       <c r="J278" s="7"/>
       <c r="K278" s="6"/>
     </row>
-    <row r="279" spans="1:11">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" s="9"/>
       <c r="B279" s="18"/>
       <c r="C279" s="19"/>
@@ -9345,7 +9358,7 @@
       <c r="J279" s="7"/>
       <c r="K279" s="6"/>
     </row>
-    <row r="280" spans="1:11">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" s="9"/>
       <c r="B280" s="18"/>
       <c r="C280" s="19"/>
@@ -9358,7 +9371,7 @@
       <c r="J280" s="7"/>
       <c r="K280" s="6"/>
     </row>
-    <row r="281" spans="1:11">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281" s="9"/>
       <c r="B281" s="18"/>
       <c r="C281" s="19"/>
@@ -9371,7 +9384,7 @@
       <c r="J281" s="7"/>
       <c r="K281" s="6"/>
     </row>
-    <row r="282" spans="1:11">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" s="9"/>
       <c r="B282" s="18"/>
       <c r="C282" s="19"/>
@@ -9384,7 +9397,7 @@
       <c r="J282" s="7"/>
       <c r="K282" s="6"/>
     </row>
-    <row r="283" spans="1:11">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283" s="9"/>
       <c r="B283" s="18"/>
       <c r="C283" s="19"/>
@@ -9397,7 +9410,7 @@
       <c r="J283" s="7"/>
       <c r="K283" s="6"/>
     </row>
-    <row r="284" spans="1:11">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" s="9"/>
       <c r="B284" s="18"/>
       <c r="C284" s="19"/>
@@ -9410,7 +9423,7 @@
       <c r="J284" s="7"/>
       <c r="K284" s="6"/>
     </row>
-    <row r="285" spans="1:11">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285" s="9"/>
       <c r="B285" s="18"/>
       <c r="C285" s="19"/>
@@ -9423,7 +9436,7 @@
       <c r="J285" s="7"/>
       <c r="K285" s="6"/>
     </row>
-    <row r="286" spans="1:11">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A286" s="9"/>
       <c r="B286" s="18"/>
       <c r="C286" s="19"/>
@@ -9436,7 +9449,7 @@
       <c r="J286" s="7"/>
       <c r="K286" s="6"/>
     </row>
-    <row r="287" spans="1:11">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A287" s="9"/>
       <c r="B287" s="18"/>
       <c r="C287" s="19"/>
@@ -9449,7 +9462,7 @@
       <c r="J287" s="7"/>
       <c r="K287" s="6"/>
     </row>
-    <row r="288" spans="1:11">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A288" s="9"/>
       <c r="B288" s="18"/>
       <c r="C288" s="19"/>
@@ -9462,7 +9475,7 @@
       <c r="J288" s="7"/>
       <c r="K288" s="6"/>
     </row>
-    <row r="289" spans="1:11">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A289" s="9"/>
       <c r="B289" s="18"/>
       <c r="C289" s="19"/>
@@ -9475,7 +9488,7 @@
       <c r="J289" s="7"/>
       <c r="K289" s="6"/>
     </row>
-    <row r="290" spans="1:11">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290" s="9"/>
       <c r="B290" s="18"/>
       <c r="C290" s="19"/>
@@ -9488,7 +9501,7 @@
       <c r="J290" s="7"/>
       <c r="K290" s="6"/>
     </row>
-    <row r="291" spans="1:11">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A291" s="9"/>
       <c r="B291" s="18"/>
       <c r="C291" s="19"/>
@@ -9501,7 +9514,7 @@
       <c r="J291" s="7"/>
       <c r="K291" s="6"/>
     </row>
-    <row r="292" spans="1:11">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A292" s="9"/>
       <c r="B292" s="18"/>
       <c r="C292" s="19"/>
@@ -9514,7 +9527,7 @@
       <c r="J292" s="7"/>
       <c r="K292" s="6"/>
     </row>
-    <row r="293" spans="1:11">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A293" s="9"/>
       <c r="B293" s="18"/>
       <c r="C293" s="19"/>
@@ -9527,7 +9540,7 @@
       <c r="J293" s="7"/>
       <c r="K293" s="6"/>
     </row>
-    <row r="294" spans="1:11">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A294" s="9"/>
       <c r="B294" s="18"/>
       <c r="C294" s="19"/>
@@ -9540,7 +9553,7 @@
       <c r="J294" s="7"/>
       <c r="K294" s="6"/>
     </row>
-    <row r="295" spans="1:11">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A295" s="9"/>
       <c r="B295" s="18"/>
       <c r="C295" s="19"/>
@@ -9553,7 +9566,7 @@
       <c r="J295" s="7"/>
       <c r="K295" s="6"/>
     </row>
-    <row r="296" spans="1:11">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A296" s="9"/>
       <c r="B296" s="18"/>
       <c r="C296" s="19"/>
@@ -9566,7 +9579,7 @@
       <c r="J296" s="7"/>
       <c r="K296" s="6"/>
     </row>
-    <row r="297" spans="1:11">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A297" s="9"/>
       <c r="B297" s="18"/>
       <c r="C297" s="19"/>
@@ -9579,7 +9592,7 @@
       <c r="J297" s="7"/>
       <c r="K297" s="6"/>
     </row>
-    <row r="298" spans="1:11">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A298" s="9"/>
       <c r="B298" s="18"/>
       <c r="C298" s="19"/>
@@ -9592,7 +9605,7 @@
       <c r="J298" s="7"/>
       <c r="K298" s="6"/>
     </row>
-    <row r="299" spans="1:11">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A299" s="9"/>
       <c r="B299" s="18"/>
       <c r="C299" s="19"/>
@@ -9605,7 +9618,7 @@
       <c r="J299" s="7"/>
       <c r="K299" s="6"/>
     </row>
-    <row r="300" spans="1:11">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A300" s="9"/>
       <c r="B300" s="18"/>
       <c r="C300" s="19"/>
@@ -9618,7 +9631,7 @@
       <c r="J300" s="7"/>
       <c r="K300" s="6"/>
     </row>
-    <row r="301" spans="1:11">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A301" s="9"/>
       <c r="B301" s="18"/>
       <c r="C301" s="19"/>
@@ -9631,7 +9644,7 @@
       <c r="J301" s="7"/>
       <c r="K301" s="6"/>
     </row>
-    <row r="302" spans="1:11">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A302" s="9"/>
       <c r="B302" s="18"/>
       <c r="C302" s="19"/>
@@ -9644,7 +9657,7 @@
       <c r="J302" s="7"/>
       <c r="K302" s="6"/>
     </row>
-    <row r="303" spans="1:11">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A303" s="9"/>
       <c r="B303" s="18"/>
       <c r="C303" s="19"/>
@@ -9657,7 +9670,7 @@
       <c r="J303" s="7"/>
       <c r="K303" s="6"/>
     </row>
-    <row r="304" spans="1:11">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A304" s="9"/>
       <c r="B304" s="18"/>
       <c r="C304" s="19"/>
@@ -9670,7 +9683,7 @@
       <c r="J304" s="7"/>
       <c r="K304" s="6"/>
     </row>
-    <row r="305" spans="1:11">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A305" s="9"/>
       <c r="B305" s="18"/>
       <c r="C305" s="19"/>
@@ -9683,7 +9696,7 @@
       <c r="J305" s="7"/>
       <c r="K305" s="6"/>
     </row>
-    <row r="306" spans="1:11">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A306" s="9"/>
       <c r="B306" s="18"/>
       <c r="C306" s="19"/>
@@ -9696,7 +9709,7 @@
       <c r="J306" s="7"/>
       <c r="K306" s="6"/>
     </row>
-    <row r="307" spans="1:11">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A307" s="9"/>
       <c r="B307" s="18"/>
       <c r="C307" s="19"/>
@@ -9709,7 +9722,7 @@
       <c r="J307" s="7"/>
       <c r="K307" s="6"/>
     </row>
-    <row r="308" spans="1:11">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A308" s="9"/>
       <c r="B308" s="18"/>
       <c r="C308" s="19"/>
@@ -9722,7 +9735,7 @@
       <c r="J308" s="7"/>
       <c r="K308" s="6"/>
     </row>
-    <row r="309" spans="1:11">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A309" s="9"/>
       <c r="B309" s="18"/>
       <c r="C309" s="19"/>
@@ -9735,7 +9748,7 @@
       <c r="J309" s="7"/>
       <c r="K309" s="6"/>
     </row>
-    <row r="310" spans="1:11">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A310" s="9"/>
       <c r="B310" s="18"/>
       <c r="C310" s="19"/>
@@ -9748,7 +9761,7 @@
       <c r="J310" s="7"/>
       <c r="K310" s="6"/>
     </row>
-    <row r="311" spans="1:11">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A311" s="9"/>
       <c r="B311" s="18"/>
       <c r="C311" s="19"/>
@@ -9761,7 +9774,7 @@
       <c r="J311" s="7"/>
       <c r="K311" s="6"/>
     </row>
-    <row r="312" spans="1:11">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A312" s="9"/>
       <c r="B312" s="18"/>
       <c r="C312" s="19"/>
@@ -9774,7 +9787,7 @@
       <c r="J312" s="7"/>
       <c r="K312" s="6"/>
     </row>
-    <row r="313" spans="1:11">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A313" s="9"/>
       <c r="B313" s="18"/>
       <c r="C313" s="19"/>
@@ -9787,7 +9800,7 @@
       <c r="J313" s="7"/>
       <c r="K313" s="6"/>
     </row>
-    <row r="314" spans="1:11">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A314" s="9"/>
       <c r="B314" s="18"/>
       <c r="C314" s="19"/>
@@ -9800,7 +9813,7 @@
       <c r="J314" s="7"/>
       <c r="K314" s="6"/>
     </row>
-    <row r="315" spans="1:11">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A315" s="9"/>
       <c r="B315" s="18"/>
       <c r="C315" s="19"/>
@@ -9813,7 +9826,7 @@
       <c r="J315" s="7"/>
       <c r="K315" s="6"/>
     </row>
-    <row r="316" spans="1:11">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A316" s="9"/>
       <c r="B316" s="18"/>
       <c r="C316" s="19"/>
@@ -9826,7 +9839,7 @@
       <c r="J316" s="7"/>
       <c r="K316" s="6"/>
     </row>
-    <row r="317" spans="1:11">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A317" s="9"/>
       <c r="B317" s="18"/>
       <c r="C317" s="19"/>
@@ -9839,7 +9852,7 @@
       <c r="J317" s="7"/>
       <c r="K317" s="6"/>
     </row>
-    <row r="318" spans="1:11">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A318" s="9"/>
       <c r="B318" s="18"/>
       <c r="C318" s="19"/>
@@ -9852,7 +9865,7 @@
       <c r="J318" s="7"/>
       <c r="K318" s="6"/>
     </row>
-    <row r="319" spans="1:11">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A319" s="9"/>
       <c r="B319" s="18"/>
       <c r="C319" s="19"/>
@@ -9865,7 +9878,7 @@
       <c r="J319" s="7"/>
       <c r="K319" s="6"/>
     </row>
-    <row r="320" spans="1:11">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A320" s="9"/>
       <c r="B320" s="18"/>
       <c r="C320" s="19"/>
@@ -9878,7 +9891,7 @@
       <c r="J320" s="7"/>
       <c r="K320" s="6"/>
     </row>
-    <row r="321" spans="1:11">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A321" s="9"/>
       <c r="B321" s="18"/>
       <c r="C321" s="19"/>
@@ -9891,7 +9904,7 @@
       <c r="J321" s="7"/>
       <c r="K321" s="6"/>
     </row>
-    <row r="322" spans="1:11">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A322" s="9"/>
       <c r="B322" s="18"/>
       <c r="C322" s="19"/>
@@ -9904,7 +9917,7 @@
       <c r="J322" s="7"/>
       <c r="K322" s="6"/>
     </row>
-    <row r="323" spans="1:11">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A323" s="9"/>
       <c r="B323" s="18"/>
       <c r="C323" s="19"/>
@@ -9917,7 +9930,7 @@
       <c r="J323" s="7"/>
       <c r="K323" s="6"/>
     </row>
-    <row r="324" spans="1:11">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324" s="9"/>
       <c r="B324" s="18"/>
       <c r="C324" s="19"/>
@@ -9930,7 +9943,7 @@
       <c r="J324" s="7"/>
       <c r="K324" s="6"/>
     </row>
-    <row r="325" spans="1:11">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A325" s="9"/>
       <c r="B325" s="18"/>
       <c r="C325" s="19"/>
@@ -9943,7 +9956,7 @@
       <c r="J325" s="7"/>
       <c r="K325" s="6"/>
     </row>
-    <row r="326" spans="1:11">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A326" s="9"/>
       <c r="B326" s="18"/>
       <c r="C326" s="19"/>
@@ -9956,7 +9969,7 @@
       <c r="J326" s="7"/>
       <c r="K326" s="6"/>
     </row>
-    <row r="327" spans="1:11">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327" s="9"/>
       <c r="B327" s="18"/>
       <c r="C327" s="19"/>
@@ -9969,7 +9982,7 @@
       <c r="J327" s="7"/>
       <c r="K327" s="6"/>
     </row>
-    <row r="328" spans="1:11">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A328" s="9"/>
       <c r="B328" s="18"/>
       <c r="C328" s="19"/>
@@ -9982,7 +9995,7 @@
       <c r="J328" s="7"/>
       <c r="K328" s="6"/>
     </row>
-    <row r="329" spans="1:11">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A329" s="9"/>
       <c r="B329" s="18"/>
       <c r="C329" s="19"/>
@@ -9995,7 +10008,7 @@
       <c r="J329" s="7"/>
       <c r="K329" s="6"/>
     </row>
-    <row r="330" spans="1:11">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A330" s="9"/>
       <c r="B330" s="18"/>
       <c r="C330" s="19"/>
@@ -10008,7 +10021,7 @@
       <c r="J330" s="7"/>
       <c r="K330" s="6"/>
     </row>
-    <row r="331" spans="1:11">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331" s="9"/>
       <c r="B331" s="18"/>
       <c r="C331" s="19"/>
@@ -10021,7 +10034,7 @@
       <c r="J331" s="7"/>
       <c r="K331" s="6"/>
     </row>
-    <row r="332" spans="1:11">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A332" s="9"/>
       <c r="B332" s="18"/>
       <c r="C332" s="19"/>
@@ -10034,7 +10047,7 @@
       <c r="J332" s="7"/>
       <c r="K332" s="6"/>
     </row>
-    <row r="333" spans="1:11">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A333" s="9"/>
       <c r="B333" s="18"/>
       <c r="C333" s="19"/>
@@ -10047,7 +10060,7 @@
       <c r="J333" s="7"/>
       <c r="K333" s="6"/>
     </row>
-    <row r="334" spans="1:11">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A334" s="9"/>
       <c r="B334" s="18"/>
       <c r="C334" s="19"/>
@@ -10060,7 +10073,7 @@
       <c r="J334" s="7"/>
       <c r="K334" s="6"/>
     </row>
-    <row r="335" spans="1:11">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A335" s="9"/>
       <c r="B335" s="18"/>
       <c r="C335" s="19"/>
@@ -10073,7 +10086,7 @@
       <c r="J335" s="7"/>
       <c r="K335" s="6"/>
     </row>
-    <row r="336" spans="1:11">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A336" s="9"/>
       <c r="B336" s="18"/>
       <c r="C336" s="19"/>
@@ -10086,7 +10099,7 @@
       <c r="J336" s="7"/>
       <c r="K336" s="6"/>
     </row>
-    <row r="337" spans="1:11">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A337" s="9"/>
       <c r="B337" s="18"/>
       <c r="C337" s="19"/>
@@ -10099,7 +10112,7 @@
       <c r="J337" s="7"/>
       <c r="K337" s="6"/>
     </row>
-    <row r="338" spans="1:11">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A338" s="9"/>
       <c r="B338" s="18"/>
       <c r="C338" s="19"/>
@@ -10112,7 +10125,7 @@
       <c r="J338" s="7"/>
       <c r="K338" s="6"/>
     </row>
-    <row r="339" spans="1:11">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A339" s="9"/>
       <c r="B339" s="18"/>
       <c r="C339" s="19"/>
@@ -10125,7 +10138,7 @@
       <c r="J339" s="7"/>
       <c r="K339" s="6"/>
     </row>
-    <row r="340" spans="1:11">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A340" s="9"/>
       <c r="B340" s="18"/>
       <c r="C340" s="19"/>
@@ -10138,7 +10151,7 @@
       <c r="J340" s="7"/>
       <c r="K340" s="6"/>
     </row>
-    <row r="341" spans="1:11">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A341" s="9"/>
       <c r="B341" s="18"/>
       <c r="C341" s="19"/>
@@ -10151,7 +10164,7 @@
       <c r="J341" s="7"/>
       <c r="K341" s="6"/>
     </row>
-    <row r="342" spans="1:11">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A342" s="9"/>
       <c r="B342" s="18"/>
       <c r="C342" s="19"/>
@@ -10164,7 +10177,7 @@
       <c r="J342" s="7"/>
       <c r="K342" s="6"/>
     </row>
-    <row r="343" spans="1:11">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A343" s="9"/>
       <c r="B343" s="18"/>
       <c r="C343" s="19"/>
@@ -10177,7 +10190,7 @@
       <c r="J343" s="7"/>
       <c r="K343" s="6"/>
     </row>
-    <row r="344" spans="1:11">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A344" s="9"/>
       <c r="B344" s="18"/>
       <c r="C344" s="19"/>
@@ -10190,7 +10203,7 @@
       <c r="J344" s="7"/>
       <c r="K344" s="6"/>
     </row>
-    <row r="345" spans="1:11">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A345" s="9"/>
       <c r="B345" s="18"/>
       <c r="C345" s="19"/>
@@ -10203,7 +10216,7 @@
       <c r="J345" s="7"/>
       <c r="K345" s="6"/>
     </row>
-    <row r="346" spans="1:11">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A346" s="9"/>
       <c r="B346" s="18"/>
       <c r="C346" s="19"/>
@@ -10216,7 +10229,7 @@
       <c r="J346" s="7"/>
       <c r="K346" s="6"/>
     </row>
-    <row r="347" spans="1:11">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A347" s="9"/>
       <c r="B347" s="18"/>
       <c r="C347" s="19"/>
@@ -10229,7 +10242,7 @@
       <c r="J347" s="7"/>
       <c r="K347" s="6"/>
     </row>
-    <row r="348" spans="1:11">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A348" s="9"/>
       <c r="B348" s="18"/>
       <c r="C348" s="19"/>
@@ -10242,7 +10255,7 @@
       <c r="J348" s="7"/>
       <c r="K348" s="6"/>
     </row>
-    <row r="349" spans="1:11">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A349" s="9"/>
       <c r="B349" s="18"/>
       <c r="C349" s="19"/>
@@ -10255,7 +10268,7 @@
       <c r="J349" s="7"/>
       <c r="K349" s="6"/>
     </row>
-    <row r="350" spans="1:11">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A350" s="9"/>
       <c r="B350" s="18"/>
       <c r="C350" s="19"/>
@@ -10268,7 +10281,7 @@
       <c r="J350" s="7"/>
       <c r="K350" s="6"/>
     </row>
-    <row r="351" spans="1:11">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A351" s="9"/>
       <c r="B351" s="18"/>
       <c r="C351" s="19"/>
@@ -10281,7 +10294,7 @@
       <c r="J351" s="7"/>
       <c r="K351" s="6"/>
     </row>
-    <row r="352" spans="1:11">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A352" s="9"/>
       <c r="B352" s="18"/>
       <c r="C352" s="19"/>
@@ -10294,7 +10307,7 @@
       <c r="J352" s="7"/>
       <c r="K352" s="6"/>
     </row>
-    <row r="353" spans="1:11">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A353" s="9"/>
       <c r="B353" s="18"/>
       <c r="C353" s="19"/>
@@ -10307,7 +10320,7 @@
       <c r="J353" s="7"/>
       <c r="K353" s="6"/>
     </row>
-    <row r="354" spans="1:11">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A354" s="9"/>
       <c r="B354" s="18"/>
       <c r="C354" s="19"/>
@@ -10320,7 +10333,7 @@
       <c r="J354" s="7"/>
       <c r="K354" s="6"/>
     </row>
-    <row r="355" spans="1:11">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A355" s="9"/>
       <c r="B355" s="18"/>
       <c r="C355" s="19"/>
@@ -10333,7 +10346,7 @@
       <c r="J355" s="7"/>
       <c r="K355" s="6"/>
     </row>
-    <row r="356" spans="1:11">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A356" s="9"/>
       <c r="B356" s="18"/>
       <c r="C356" s="19"/>
@@ -10346,7 +10359,7 @@
       <c r="J356" s="7"/>
       <c r="K356" s="6"/>
     </row>
-    <row r="357" spans="1:11">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A357" s="9"/>
       <c r="B357" s="18"/>
       <c r="C357" s="19"/>
@@ -10359,7 +10372,7 @@
       <c r="J357" s="7"/>
       <c r="K357" s="6"/>
     </row>
-    <row r="358" spans="1:11">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A358" s="9"/>
       <c r="B358" s="18"/>
       <c r="C358" s="19"/>
@@ -10372,7 +10385,7 @@
       <c r="J358" s="7"/>
       <c r="K358" s="6"/>
     </row>
-    <row r="359" spans="1:11">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A359" s="9"/>
       <c r="B359" s="18"/>
       <c r="C359" s="19"/>
@@ -10385,7 +10398,7 @@
       <c r="J359" s="7"/>
       <c r="K359" s="6"/>
     </row>
-    <row r="360" spans="1:11">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A360" s="9"/>
       <c r="B360" s="18"/>
       <c r="C360" s="19"/>
@@ -10398,7 +10411,7 @@
       <c r="J360" s="7"/>
       <c r="K360" s="6"/>
     </row>
-    <row r="361" spans="1:11">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A361" s="9"/>
       <c r="B361" s="18"/>
       <c r="C361" s="19"/>
@@ -10411,7 +10424,7 @@
       <c r="J361" s="7"/>
       <c r="K361" s="6"/>
     </row>
-    <row r="362" spans="1:11">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A362" s="9"/>
       <c r="B362" s="18"/>
       <c r="C362" s="19"/>
@@ -10424,7 +10437,7 @@
       <c r="J362" s="7"/>
       <c r="K362" s="6"/>
     </row>
-    <row r="363" spans="1:11">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A363" s="9"/>
       <c r="B363" s="18"/>
       <c r="C363" s="19"/>
@@ -10437,7 +10450,7 @@
       <c r="J363" s="7"/>
       <c r="K363" s="6"/>
     </row>
-    <row r="364" spans="1:11">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A364" s="9"/>
       <c r="B364" s="18"/>
       <c r="C364" s="19"/>
@@ -10450,7 +10463,7 @@
       <c r="J364" s="7"/>
       <c r="K364" s="6"/>
     </row>
-    <row r="365" spans="1:11">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A365" s="9"/>
       <c r="B365" s="18"/>
       <c r="C365" s="19"/>
@@ -10463,7 +10476,7 @@
       <c r="J365" s="7"/>
       <c r="K365" s="6"/>
     </row>
-    <row r="366" spans="1:11">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A366" s="9"/>
       <c r="B366" s="18"/>
       <c r="C366" s="19"/>
@@ -10476,7 +10489,7 @@
       <c r="J366" s="7"/>
       <c r="K366" s="6"/>
     </row>
-    <row r="367" spans="1:11">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A367" s="9"/>
       <c r="B367" s="18"/>
       <c r="C367" s="19"/>
@@ -10489,7 +10502,7 @@
       <c r="J367" s="7"/>
       <c r="K367" s="6"/>
     </row>
-    <row r="368" spans="1:11">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A368" s="9"/>
       <c r="B368" s="18"/>
       <c r="C368" s="19"/>
@@ -10502,7 +10515,7 @@
       <c r="J368" s="7"/>
       <c r="K368" s="6"/>
     </row>
-    <row r="369" spans="1:11">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A369" s="9"/>
       <c r="B369" s="18"/>
       <c r="C369" s="19"/>
@@ -10515,7 +10528,7 @@
       <c r="J369" s="7"/>
       <c r="K369" s="6"/>
     </row>
-    <row r="370" spans="1:11">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A370" s="9"/>
       <c r="B370" s="18"/>
       <c r="C370" s="19"/>
@@ -10528,7 +10541,7 @@
       <c r="J370" s="7"/>
       <c r="K370" s="6"/>
     </row>
-    <row r="371" spans="1:11">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A371" s="9"/>
       <c r="B371" s="18"/>
       <c r="C371" s="19"/>
@@ -10541,7 +10554,7 @@
       <c r="J371" s="7"/>
       <c r="K371" s="6"/>
     </row>
-    <row r="372" spans="1:11">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A372" s="9"/>
       <c r="B372" s="18"/>
       <c r="C372" s="19"/>
@@ -10554,7 +10567,7 @@
       <c r="J372" s="7"/>
       <c r="K372" s="6"/>
     </row>
-    <row r="373" spans="1:11">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A373" s="9"/>
       <c r="B373" s="18"/>
       <c r="C373" s="19"/>
@@ -10567,7 +10580,7 @@
       <c r="J373" s="7"/>
       <c r="K373" s="6"/>
     </row>
-    <row r="374" spans="1:11">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A374" s="9"/>
       <c r="B374" s="18"/>
       <c r="C374" s="19"/>
@@ -10580,7 +10593,7 @@
       <c r="J374" s="7"/>
       <c r="K374" s="6"/>
     </row>
-    <row r="375" spans="1:11">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A375" s="9"/>
       <c r="B375" s="18"/>
       <c r="C375" s="19"/>
@@ -10593,7 +10606,7 @@
       <c r="J375" s="7"/>
       <c r="K375" s="6"/>
     </row>
-    <row r="376" spans="1:11">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A376" s="9"/>
       <c r="B376" s="18"/>
       <c r="C376" s="19"/>
@@ -10606,7 +10619,7 @@
       <c r="J376" s="7"/>
       <c r="K376" s="6"/>
     </row>
-    <row r="377" spans="1:11">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A377" s="9"/>
       <c r="B377" s="18"/>
       <c r="C377" s="19"/>
@@ -10619,7 +10632,7 @@
       <c r="J377" s="7"/>
       <c r="K377" s="6"/>
     </row>
-    <row r="378" spans="1:11">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A378" s="9"/>
       <c r="B378" s="18"/>
       <c r="C378" s="19"/>
@@ -10632,7 +10645,7 @@
       <c r="J378" s="7"/>
       <c r="K378" s="6"/>
     </row>
-    <row r="379" spans="1:11">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A379" s="9"/>
       <c r="B379" s="18"/>
       <c r="C379" s="19"/>
@@ -10645,7 +10658,7 @@
       <c r="J379" s="7"/>
       <c r="K379" s="6"/>
     </row>
-    <row r="380" spans="1:11">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A380" s="9"/>
       <c r="B380" s="18"/>
       <c r="C380" s="19"/>
@@ -10658,7 +10671,7 @@
       <c r="J380" s="7"/>
       <c r="K380" s="6"/>
     </row>
-    <row r="381" spans="1:11">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A381" s="9"/>
       <c r="B381" s="18"/>
       <c r="C381" s="19"/>
@@ -10671,7 +10684,7 @@
       <c r="J381" s="7"/>
       <c r="K381" s="6"/>
     </row>
-    <row r="382" spans="1:11">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A382" s="9"/>
       <c r="B382" s="18"/>
       <c r="C382" s="19"/>
@@ -10684,7 +10697,7 @@
       <c r="J382" s="7"/>
       <c r="K382" s="6"/>
     </row>
-    <row r="383" spans="1:11">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A383" s="9"/>
       <c r="B383" s="18"/>
       <c r="C383" s="19"/>
@@ -10697,7 +10710,7 @@
       <c r="J383" s="7"/>
       <c r="K383" s="6"/>
     </row>
-    <row r="384" spans="1:11">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A384" s="9"/>
       <c r="B384" s="18"/>
       <c r="C384" s="19"/>
@@ -10710,7 +10723,7 @@
       <c r="J384" s="7"/>
       <c r="K384" s="6"/>
     </row>
-    <row r="385" spans="1:11">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A385" s="9"/>
       <c r="B385" s="18"/>
       <c r="C385" s="19"/>
@@ -10723,7 +10736,7 @@
       <c r="J385" s="7"/>
       <c r="K385" s="6"/>
     </row>
-    <row r="386" spans="1:11">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A386" s="9"/>
       <c r="B386" s="18"/>
       <c r="C386" s="19"/>
@@ -10736,7 +10749,7 @@
       <c r="J386" s="7"/>
       <c r="K386" s="6"/>
     </row>
-    <row r="387" spans="1:11">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A387" s="9"/>
       <c r="B387" s="18"/>
       <c r="C387" s="19"/>
@@ -10749,7 +10762,7 @@
       <c r="J387" s="7"/>
       <c r="K387" s="6"/>
     </row>
-    <row r="388" spans="1:11">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A388" s="9"/>
       <c r="B388" s="18"/>
       <c r="C388" s="19"/>
@@ -10762,7 +10775,7 @@
       <c r="J388" s="7"/>
       <c r="K388" s="6"/>
     </row>
-    <row r="389" spans="1:11">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A389" s="9"/>
       <c r="B389" s="18"/>
       <c r="C389" s="19"/>
@@ -10775,7 +10788,7 @@
       <c r="J389" s="7"/>
       <c r="K389" s="6"/>
     </row>
-    <row r="390" spans="1:11">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A390" s="9"/>
       <c r="B390" s="18"/>
       <c r="C390" s="19"/>
@@ -10788,7 +10801,7 @@
       <c r="J390" s="7"/>
       <c r="K390" s="6"/>
     </row>
-    <row r="391" spans="1:11">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A391" s="9"/>
       <c r="B391" s="18"/>
       <c r="C391" s="19"/>
@@ -10801,7 +10814,7 @@
       <c r="J391" s="7"/>
       <c r="K391" s="6"/>
     </row>
-    <row r="392" spans="1:11">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A392" s="9"/>
       <c r="B392" s="18"/>
       <c r="C392" s="19"/>
@@ -10814,7 +10827,7 @@
       <c r="J392" s="7"/>
       <c r="K392" s="6"/>
     </row>
-    <row r="393" spans="1:11">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A393" s="9"/>
       <c r="B393" s="18"/>
       <c r="C393" s="19"/>
@@ -10827,7 +10840,7 @@
       <c r="J393" s="7"/>
       <c r="K393" s="6"/>
     </row>
-    <row r="394" spans="1:11">
+    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A394" s="9"/>
       <c r="B394" s="18"/>
       <c r="C394" s="19"/>
@@ -10840,7 +10853,7 @@
       <c r="J394" s="7"/>
       <c r="K394" s="6"/>
     </row>
-    <row r="395" spans="1:11">
+    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A395" s="9"/>
       <c r="B395" s="18"/>
       <c r="C395" s="19"/>
@@ -10853,7 +10866,7 @@
       <c r="J395" s="7"/>
       <c r="K395" s="6"/>
     </row>
-    <row r="396" spans="1:11">
+    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A396" s="9"/>
       <c r="B396" s="18"/>
       <c r="C396" s="19"/>
@@ -10866,7 +10879,7 @@
       <c r="J396" s="7"/>
       <c r="K396" s="6"/>
     </row>
-    <row r="397" spans="1:11">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A397" s="9"/>
       <c r="B397" s="18"/>
       <c r="C397" s="19"/>
@@ -10879,7 +10892,7 @@
       <c r="J397" s="7"/>
       <c r="K397" s="6"/>
     </row>
-    <row r="398" spans="1:11">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A398" s="9"/>
       <c r="B398" s="18"/>
       <c r="C398" s="19"/>
@@ -10892,7 +10905,7 @@
       <c r="J398" s="7"/>
       <c r="K398" s="6"/>
     </row>
-    <row r="399" spans="1:11">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A399" s="9"/>
       <c r="B399" s="18"/>
       <c r="C399" s="19"/>
@@ -10905,7 +10918,7 @@
       <c r="J399" s="7"/>
       <c r="K399" s="6"/>
     </row>
-    <row r="400" spans="1:11">
+    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A400" s="9"/>
       <c r="B400" s="18"/>
       <c r="C400" s="19"/>
@@ -10918,7 +10931,7 @@
       <c r="J400" s="7"/>
       <c r="K400" s="6"/>
     </row>
-    <row r="401" spans="1:11">
+    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A401" s="9"/>
       <c r="B401" s="18"/>
       <c r="C401" s="19"/>
@@ -10931,7 +10944,7 @@
       <c r="J401" s="7"/>
       <c r="K401" s="6"/>
     </row>
-    <row r="402" spans="1:11">
+    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A402" s="9"/>
       <c r="B402" s="18"/>
       <c r="C402" s="19"/>
@@ -10944,7 +10957,7 @@
       <c r="J402" s="7"/>
       <c r="K402" s="6"/>
     </row>
-    <row r="403" spans="1:11">
+    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A403" s="9"/>
       <c r="B403" s="18"/>
       <c r="C403" s="19"/>
@@ -10957,7 +10970,7 @@
       <c r="J403" s="7"/>
       <c r="K403" s="6"/>
     </row>
-    <row r="404" spans="1:11">
+    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A404" s="9"/>
       <c r="B404" s="18"/>
       <c r="C404" s="19"/>
@@ -10970,7 +10983,7 @@
       <c r="J404" s="7"/>
       <c r="K404" s="6"/>
     </row>
-    <row r="405" spans="1:11">
+    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A405" s="19"/>
       <c r="B405" s="18"/>
       <c r="C405" s="19"/>
@@ -10983,7 +10996,7 @@
       <c r="J405" s="7"/>
       <c r="K405" s="6"/>
     </row>
-    <row r="406" spans="1:11">
+    <row r="406" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A406" s="19"/>
       <c r="B406" s="18"/>
       <c r="C406" s="19"/>
@@ -10996,7 +11009,7 @@
       <c r="J406" s="7"/>
       <c r="K406" s="6"/>
     </row>
-    <row r="407" spans="1:11">
+    <row r="407" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A407" s="19"/>
       <c r="B407" s="18"/>
       <c r="C407" s="19"/>
@@ -11009,7 +11022,7 @@
       <c r="J407" s="7"/>
       <c r="K407" s="6"/>
     </row>
-    <row r="408" spans="1:11">
+    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A408" s="19"/>
       <c r="B408" s="18"/>
       <c r="C408" s="19"/>
@@ -11022,7 +11035,7 @@
       <c r="J408" s="7"/>
       <c r="K408" s="6"/>
     </row>
-    <row r="409" spans="1:11">
+    <row r="409" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A409" s="19"/>
       <c r="B409" s="18"/>
       <c r="C409" s="19"/>
@@ -11035,7 +11048,7 @@
       <c r="J409" s="7"/>
       <c r="K409" s="6"/>
     </row>
-    <row r="410" spans="1:11">
+    <row r="410" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A410" s="19"/>
       <c r="B410" s="18"/>
       <c r="C410" s="19"/>
@@ -11048,7 +11061,7 @@
       <c r="J410" s="7"/>
       <c r="K410" s="6"/>
     </row>
-    <row r="411" spans="1:11">
+    <row r="411" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A411" s="19"/>
       <c r="B411" s="18"/>
       <c r="C411" s="19"/>
@@ -11061,7 +11074,7 @@
       <c r="J411" s="7"/>
       <c r="K411" s="6"/>
     </row>
-    <row r="412" spans="1:11">
+    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A412" s="19"/>
       <c r="B412" s="18"/>
       <c r="C412" s="19"/>
@@ -11074,7 +11087,7 @@
       <c r="J412" s="7"/>
       <c r="K412" s="6"/>
     </row>
-    <row r="413" spans="1:11">
+    <row r="413" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A413" s="19"/>
       <c r="B413" s="18"/>
       <c r="C413" s="19"/>
@@ -11087,7 +11100,7 @@
       <c r="J413" s="7"/>
       <c r="K413" s="6"/>
     </row>
-    <row r="414" spans="1:11">
+    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A414" s="19"/>
       <c r="B414" s="18"/>
       <c r="C414" s="19"/>
@@ -11100,7 +11113,7 @@
       <c r="J414" s="7"/>
       <c r="K414" s="6"/>
     </row>
-    <row r="415" spans="1:11">
+    <row r="415" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A415" s="19"/>
       <c r="B415" s="18"/>
       <c r="C415" s="19"/>
@@ -11113,7 +11126,7 @@
       <c r="J415" s="7"/>
       <c r="K415" s="6"/>
     </row>
-    <row r="416" spans="1:11">
+    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A416" s="19"/>
       <c r="B416" s="18"/>
       <c r="C416" s="19"/>
@@ -11126,7 +11139,7 @@
       <c r="J416" s="7"/>
       <c r="K416" s="6"/>
     </row>
-    <row r="417" spans="1:11">
+    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A417" s="19"/>
       <c r="B417" s="18"/>
       <c r="C417" s="19"/>
@@ -11139,7 +11152,7 @@
       <c r="J417" s="7"/>
       <c r="K417" s="6"/>
     </row>
-    <row r="418" spans="1:11">
+    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A418" s="19"/>
       <c r="B418" s="18"/>
       <c r="C418" s="19"/>
@@ -11152,7 +11165,7 @@
       <c r="J418" s="7"/>
       <c r="K418" s="6"/>
     </row>
-    <row r="419" spans="1:11">
+    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A419" s="19"/>
       <c r="B419" s="18"/>
       <c r="C419" s="19"/>
@@ -11165,7 +11178,7 @@
       <c r="J419" s="7"/>
       <c r="K419" s="6"/>
     </row>
-    <row r="420" spans="1:11">
+    <row r="420" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A420" s="19"/>
       <c r="B420" s="18"/>
       <c r="C420" s="19"/>
@@ -11178,7 +11191,7 @@
       <c r="J420" s="7"/>
       <c r="K420" s="6"/>
     </row>
-    <row r="421" spans="1:11">
+    <row r="421" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A421" s="19"/>
       <c r="B421" s="18"/>
       <c r="C421" s="19"/>
@@ -11191,7 +11204,7 @@
       <c r="J421" s="7"/>
       <c r="K421" s="6"/>
     </row>
-    <row r="422" spans="1:11">
+    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A422" s="19"/>
       <c r="B422" s="18"/>
       <c r="C422" s="19"/>
@@ -11204,7 +11217,7 @@
       <c r="J422" s="7"/>
       <c r="K422" s="6"/>
     </row>
-    <row r="423" spans="1:11">
+    <row r="423" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A423" s="19"/>
       <c r="B423" s="18"/>
       <c r="C423" s="19"/>
@@ -11217,7 +11230,7 @@
       <c r="J423" s="7"/>
       <c r="K423" s="6"/>
     </row>
-    <row r="424" spans="1:11">
+    <row r="424" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A424" s="19"/>
       <c r="B424" s="18"/>
       <c r="C424" s="19"/>
@@ -11230,7 +11243,7 @@
       <c r="J424" s="7"/>
       <c r="K424" s="6"/>
     </row>
-    <row r="425" spans="1:11">
+    <row r="425" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A425" s="19"/>
       <c r="B425" s="18"/>
       <c r="C425" s="19"/>
@@ -11243,7 +11256,7 @@
       <c r="J425" s="7"/>
       <c r="K425" s="6"/>
     </row>
-    <row r="426" spans="1:11">
+    <row r="426" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A426" s="19"/>
       <c r="B426" s="18"/>
       <c r="C426" s="19"/>
@@ -11256,7 +11269,7 @@
       <c r="J426" s="7"/>
       <c r="K426" s="6"/>
     </row>
-    <row r="427" spans="1:11">
+    <row r="427" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A427" s="19"/>
       <c r="B427" s="18"/>
       <c r="C427" s="19"/>
@@ -11269,7 +11282,7 @@
       <c r="J427" s="7"/>
       <c r="K427" s="6"/>
     </row>
-    <row r="428" spans="1:11">
+    <row r="428" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A428" s="19"/>
       <c r="B428" s="18"/>
       <c r="C428" s="19"/>
@@ -11282,7 +11295,7 @@
       <c r="J428" s="7"/>
       <c r="K428" s="6"/>
     </row>
-    <row r="429" spans="1:11">
+    <row r="429" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A429" s="19"/>
       <c r="B429" s="18"/>
       <c r="C429" s="19"/>
@@ -11295,7 +11308,7 @@
       <c r="J429" s="7"/>
       <c r="K429" s="6"/>
     </row>
-    <row r="430" spans="1:11">
+    <row r="430" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A430" s="19"/>
       <c r="B430" s="18"/>
       <c r="C430" s="19"/>
@@ -11308,7 +11321,7 @@
       <c r="J430" s="7"/>
       <c r="K430" s="6"/>
     </row>
-    <row r="431" spans="1:11">
+    <row r="431" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A431" s="19"/>
       <c r="B431" s="18"/>
       <c r="C431" s="19"/>
@@ -11321,7 +11334,7 @@
       <c r="J431" s="7"/>
       <c r="K431" s="6"/>
     </row>
-    <row r="432" spans="1:11">
+    <row r="432" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A432" s="19"/>
       <c r="B432" s="18"/>
       <c r="C432" s="19"/>
@@ -11334,7 +11347,7 @@
       <c r="J432" s="7"/>
       <c r="K432" s="6"/>
     </row>
-    <row r="433" spans="1:11">
+    <row r="433" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A433" s="19"/>
       <c r="B433" s="18"/>
       <c r="C433" s="19"/>
@@ -11347,7 +11360,7 @@
       <c r="J433" s="7"/>
       <c r="K433" s="6"/>
     </row>
-    <row r="434" spans="1:11">
+    <row r="434" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A434" s="19"/>
       <c r="B434" s="18"/>
       <c r="C434" s="19"/>
@@ -11360,7 +11373,7 @@
       <c r="J434" s="7"/>
       <c r="K434" s="6"/>
     </row>
-    <row r="435" spans="1:11">
+    <row r="435" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A435" s="19"/>
       <c r="B435" s="18"/>
       <c r="C435" s="19"/>
@@ -11373,7 +11386,7 @@
       <c r="J435" s="7"/>
       <c r="K435" s="6"/>
     </row>
-    <row r="436" spans="1:11">
+    <row r="436" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A436" s="19"/>
       <c r="B436" s="18"/>
       <c r="C436" s="19"/>
@@ -11386,7 +11399,7 @@
       <c r="J436" s="7"/>
       <c r="K436" s="6"/>
     </row>
-    <row r="437" spans="1:11">
+    <row r="437" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A437" s="19"/>
       <c r="B437" s="18"/>
       <c r="C437" s="19"/>
@@ -11399,7 +11412,7 @@
       <c r="J437" s="7"/>
       <c r="K437" s="6"/>
     </row>
-    <row r="438" spans="1:11">
+    <row r="438" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A438" s="19"/>
       <c r="B438" s="18"/>
       <c r="C438" s="19"/>
@@ -11412,7 +11425,7 @@
       <c r="J438" s="7"/>
       <c r="K438" s="6"/>
     </row>
-    <row r="439" spans="1:11">
+    <row r="439" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A439" s="19"/>
       <c r="B439" s="18"/>
       <c r="C439" s="19"/>
@@ -11425,7 +11438,7 @@
       <c r="J439" s="7"/>
       <c r="K439" s="6"/>
     </row>
-    <row r="440" spans="1:11">
+    <row r="440" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A440" s="19"/>
       <c r="B440" s="18"/>
       <c r="C440" s="19"/>
@@ -11438,7 +11451,7 @@
       <c r="J440" s="7"/>
       <c r="K440" s="6"/>
     </row>
-    <row r="441" spans="1:11">
+    <row r="441" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A441" s="19"/>
       <c r="B441" s="18"/>
       <c r="C441" s="19"/>
@@ -11451,7 +11464,7 @@
       <c r="J441" s="7"/>
       <c r="K441" s="6"/>
     </row>
-    <row r="442" spans="1:11">
+    <row r="442" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A442" s="19"/>
       <c r="B442" s="18"/>
       <c r="C442" s="19"/>
@@ -11464,7 +11477,7 @@
       <c r="J442" s="7"/>
       <c r="K442" s="6"/>
     </row>
-    <row r="443" spans="1:11">
+    <row r="443" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A443" s="19"/>
       <c r="B443" s="18"/>
       <c r="C443" s="19"/>
@@ -11477,7 +11490,7 @@
       <c r="J443" s="7"/>
       <c r="K443" s="6"/>
     </row>
-    <row r="444" spans="1:11">
+    <row r="444" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A444" s="19"/>
       <c r="B444" s="18"/>
       <c r="C444" s="19"/>
@@ -11490,7 +11503,7 @@
       <c r="J444" s="7"/>
       <c r="K444" s="6"/>
     </row>
-    <row r="445" spans="1:11">
+    <row r="445" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A445" s="19"/>
       <c r="B445" s="18"/>
       <c r="C445" s="19"/>
@@ -11503,7 +11516,7 @@
       <c r="J445" s="7"/>
       <c r="K445" s="6"/>
     </row>
-    <row r="446" spans="1:11">
+    <row r="446" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A446" s="19"/>
       <c r="B446" s="18"/>
       <c r="C446" s="19"/>
@@ -11516,7 +11529,7 @@
       <c r="J446" s="7"/>
       <c r="K446" s="6"/>
     </row>
-    <row r="447" spans="1:11">
+    <row r="447" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A447" s="19"/>
       <c r="B447" s="18"/>
       <c r="C447" s="19"/>
@@ -11529,7 +11542,7 @@
       <c r="J447" s="7"/>
       <c r="K447" s="6"/>
     </row>
-    <row r="448" spans="1:11">
+    <row r="448" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A448" s="19"/>
       <c r="B448" s="18"/>
       <c r="C448" s="19"/>
@@ -11542,7 +11555,7 @@
       <c r="J448" s="7"/>
       <c r="K448" s="6"/>
     </row>
-    <row r="449" spans="1:11">
+    <row r="449" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A449" s="19"/>
       <c r="B449" s="18"/>
       <c r="C449" s="19"/>
@@ -11555,7 +11568,7 @@
       <c r="J449" s="7"/>
       <c r="K449" s="6"/>
     </row>
-    <row r="450" spans="1:11">
+    <row r="450" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A450" s="19"/>
       <c r="B450" s="18"/>
       <c r="C450" s="19"/>
@@ -11568,7 +11581,7 @@
       <c r="J450" s="7"/>
       <c r="K450" s="6"/>
     </row>
-    <row r="451" spans="1:11">
+    <row r="451" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A451" s="19"/>
       <c r="B451" s="18"/>
       <c r="C451" s="19"/>
@@ -11581,7 +11594,7 @@
       <c r="J451" s="7"/>
       <c r="K451" s="6"/>
     </row>
-    <row r="452" spans="1:11">
+    <row r="452" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A452" s="19"/>
       <c r="B452" s="18"/>
       <c r="C452" s="19"/>
@@ -11594,7 +11607,7 @@
       <c r="J452" s="7"/>
       <c r="K452" s="6"/>
     </row>
-    <row r="453" spans="1:11">
+    <row r="453" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A453" s="19"/>
       <c r="B453" s="18"/>
       <c r="C453" s="19"/>
@@ -11607,7 +11620,7 @@
       <c r="J453" s="7"/>
       <c r="K453" s="6"/>
     </row>
-    <row r="454" spans="1:11">
+    <row r="454" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A454" s="19"/>
       <c r="B454" s="18"/>
       <c r="C454" s="19"/>
@@ -11620,7 +11633,7 @@
       <c r="J454" s="7"/>
       <c r="K454" s="6"/>
     </row>
-    <row r="455" spans="1:11">
+    <row r="455" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A455" s="19"/>
       <c r="B455" s="18"/>
       <c r="C455" s="19"/>
@@ -11633,7 +11646,7 @@
       <c r="J455" s="7"/>
       <c r="K455" s="6"/>
     </row>
-    <row r="456" spans="1:11">
+    <row r="456" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A456" s="19"/>
       <c r="B456" s="18"/>
       <c r="C456" s="19"/>
@@ -11646,7 +11659,7 @@
       <c r="J456" s="7"/>
       <c r="K456" s="6"/>
     </row>
-    <row r="457" spans="1:11">
+    <row r="457" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A457" s="19"/>
       <c r="B457" s="18"/>
       <c r="C457" s="19"/>
@@ -11659,7 +11672,7 @@
       <c r="J457" s="7"/>
       <c r="K457" s="6"/>
     </row>
-    <row r="458" spans="1:11">
+    <row r="458" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A458" s="19"/>
       <c r="B458" s="18"/>
       <c r="C458" s="19"/>
@@ -11672,7 +11685,7 @@
       <c r="J458" s="7"/>
       <c r="K458" s="6"/>
     </row>
-    <row r="459" spans="1:11">
+    <row r="459" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A459" s="19"/>
       <c r="B459" s="18"/>
       <c r="C459" s="19"/>
@@ -11685,7 +11698,7 @@
       <c r="J459" s="7"/>
       <c r="K459" s="6"/>
     </row>
-    <row r="460" spans="1:11">
+    <row r="460" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A460" s="19"/>
       <c r="B460" s="18"/>
       <c r="C460" s="19"/>
@@ -11698,7 +11711,7 @@
       <c r="J460" s="7"/>
       <c r="K460" s="6"/>
     </row>
-    <row r="461" spans="1:11">
+    <row r="461" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A461" s="19"/>
       <c r="B461" s="18"/>
       <c r="C461" s="19"/>
@@ -11711,7 +11724,7 @@
       <c r="J461" s="7"/>
       <c r="K461" s="6"/>
     </row>
-    <row r="462" spans="1:11">
+    <row r="462" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A462" s="19"/>
       <c r="B462" s="18"/>
       <c r="C462" s="19"/>
@@ -11724,7 +11737,7 @@
       <c r="J462" s="7"/>
       <c r="K462" s="6"/>
     </row>
-    <row r="463" spans="1:11">
+    <row r="463" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A463" s="19"/>
       <c r="B463" s="18"/>
       <c r="C463" s="19"/>
@@ -11737,7 +11750,7 @@
       <c r="J463" s="7"/>
       <c r="K463" s="6"/>
     </row>
-    <row r="464" spans="1:11">
+    <row r="464" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A464" s="19"/>
       <c r="B464" s="18"/>
       <c r="C464" s="19"/>
@@ -11750,7 +11763,7 @@
       <c r="J464" s="7"/>
       <c r="K464" s="6"/>
     </row>
-    <row r="465" spans="1:11">
+    <row r="465" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A465" s="19"/>
       <c r="B465" s="18"/>
       <c r="C465" s="19"/>
@@ -11763,7 +11776,7 @@
       <c r="J465" s="7"/>
       <c r="K465" s="6"/>
     </row>
-    <row r="466" spans="1:11">
+    <row r="466" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A466" s="19"/>
       <c r="B466" s="18"/>
       <c r="C466" s="19"/>
@@ -11776,7 +11789,7 @@
       <c r="J466" s="7"/>
       <c r="K466" s="6"/>
     </row>
-    <row r="467" spans="1:11">
+    <row r="467" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A467" s="19"/>
       <c r="B467" s="18"/>
       <c r="C467" s="19"/>
@@ -11789,7 +11802,7 @@
       <c r="J467" s="7"/>
       <c r="K467" s="6"/>
     </row>
-    <row r="468" spans="1:11">
+    <row r="468" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A468" s="19"/>
       <c r="B468" s="18"/>
       <c r="C468" s="19"/>
@@ -11802,7 +11815,7 @@
       <c r="J468" s="7"/>
       <c r="K468" s="6"/>
     </row>
-    <row r="469" spans="1:11">
+    <row r="469" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A469" s="19"/>
       <c r="B469" s="18"/>
       <c r="C469" s="19"/>
@@ -11821,6 +11834,9 @@
     <mergeCell ref="J1:J3"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{58DDAF71-A1E9-444F-9179-E77870B02596}"/>
     <hyperlink ref="D6" r:id="rId2" xr:uid="{463EAD0E-9251-4782-B20B-89F75D0D3F1B}"/>

</xml_diff>